<commit_message>
add espindola schedule of campus 'oyon'
</commit_message>
<xml_diff>
--- a/data/horarios/horarios.sedes.raw.xlsx
+++ b/data/horarios/horarios.sedes.raw.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\Documents\GitHub\fcc-pregrado-horarios-y-matriculas-xlsx-to-json\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\Documents\GitHub\fcc-pregrado-horarios-y-matriculas-xlsx-to-json\data\horarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC37151-0ABB-4BE3-A836-3248A1B65AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2177A0D0-D162-4073-9513-55E1D58C5320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -199,9 +199,6 @@
     <t>VELÁSQUEZ MEDINA, MARTÍN</t>
   </si>
   <si>
-    <t>ESPÍNDOLA ARMANDO</t>
-  </si>
-  <si>
     <t>08.45-12.30</t>
   </si>
   <si>
@@ -230,6 +227,9 @@
   </si>
   <si>
     <t>PALACIOS DÍAZ, CYNTHIA MILAGROS</t>
+  </si>
+  <si>
+    <t>ESPINDOLA MILLA ARMANDO JUNIOR</t>
   </si>
 </sst>
 </file>
@@ -725,7 +725,7 @@
   <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,7 +814,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D2" s="12">
         <v>111142</v>
@@ -835,7 +835,7 @@
         <v>3</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K2" s="14" t="s">
         <v>19</v>
@@ -844,7 +844,7 @@
         <v>48</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N2" s="14"/>
       <c r="O2" s="14"/>
@@ -860,7 +860,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3" s="12">
         <v>111143</v>
@@ -881,7 +881,7 @@
         <v>3</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K3" s="14" t="s">
         <v>19</v>
@@ -891,7 +891,7 @@
       </c>
       <c r="M3" s="16"/>
       <c r="N3" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O3" s="14"/>
       <c r="P3" s="14"/>
@@ -906,7 +906,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" s="12">
         <v>111144</v>
@@ -927,7 +927,7 @@
         <v>3</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K4" s="14" t="s">
         <v>32</v>
@@ -952,7 +952,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D5" s="12">
         <v>111145</v>
@@ -973,7 +973,7 @@
         <v>3</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K5" s="14" t="s">
         <v>19</v>
@@ -998,7 +998,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D6" s="12">
         <v>111146</v>
@@ -1019,7 +1019,7 @@
         <v>3</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K6" s="14" t="s">
         <v>19</v>
@@ -1032,7 +1032,7 @@
       <c r="O6" s="16"/>
       <c r="P6" s="14"/>
       <c r="Q6" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="R6" s="14"/>
     </row>
@@ -1044,7 +1044,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" s="12">
         <v>111147</v>
@@ -1065,13 +1065,13 @@
         <v>3</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K7" s="14" t="s">
         <v>32</v>
       </c>
       <c r="L7" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M7" s="14"/>
       <c r="N7" s="14"/>
@@ -1082,7 +1082,7 @@
       </c>
       <c r="R7" s="14"/>
     </row>
-    <row r="8" spans="1:18" ht="33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="66" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>2022</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8" s="12">
         <v>111148</v>
@@ -1111,19 +1111,19 @@
         <v>3</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K8" s="8" t="s">
         <v>19</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
       <c r="P8" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q8" s="10"/>
       <c r="R8" s="8"/>
@@ -1136,7 +1136,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" s="12">
         <v>111149</v>
@@ -1157,13 +1157,13 @@
         <v>3</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K9" s="14" t="s">
         <v>32</v>
       </c>
       <c r="L9" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M9" s="14"/>
       <c r="N9" s="14"/>
@@ -1276,7 +1276,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D2" s="12">
         <v>111142</v>
@@ -1297,7 +1297,7 @@
         <v>3</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K2" s="14" t="s">
         <v>19</v>
@@ -1322,7 +1322,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3" s="12">
         <v>111143</v>
@@ -1343,7 +1343,7 @@
         <v>3</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K3" s="14" t="s">
         <v>19</v>
@@ -1368,7 +1368,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" s="12">
         <v>111144</v>
@@ -1389,7 +1389,7 @@
         <v>3</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K4" s="14" t="s">
         <v>19</v>
@@ -1414,7 +1414,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D5" s="12">
         <v>111145</v>
@@ -1435,7 +1435,7 @@
         <v>3</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K5" s="14" t="s">
         <v>19</v>
@@ -1460,7 +1460,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D6" s="12">
         <v>111146</v>
@@ -1481,7 +1481,7 @@
         <v>3</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K6" s="14" t="s">
         <v>19</v>
@@ -1506,7 +1506,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" s="12">
         <v>111147</v>
@@ -1527,7 +1527,7 @@
         <v>3</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K7" s="14" t="s">
         <v>32</v>
@@ -1552,7 +1552,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8" s="12">
         <v>111148</v>
@@ -1573,7 +1573,7 @@
         <v>3</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K8" s="14" t="s">
         <v>19</v>
@@ -1598,7 +1598,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" s="12">
         <v>111149</v>
@@ -1619,7 +1619,7 @@
         <v>3</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K9" s="14" t="s">
         <v>19</v>
@@ -1741,7 +1741,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D2" s="12">
         <v>111142</v>
@@ -1762,7 +1762,7 @@
         <v>3</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K2" s="14" t="s">
         <v>19</v>
@@ -1787,7 +1787,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3" s="12">
         <v>111143</v>
@@ -1808,7 +1808,7 @@
         <v>3</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K3" s="14" t="s">
         <v>19</v>
@@ -1833,7 +1833,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" s="12">
         <v>111144</v>
@@ -1854,7 +1854,7 @@
         <v>3</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K4" s="14" t="s">
         <v>19</v>
@@ -1879,7 +1879,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D5" s="12">
         <v>111145</v>
@@ -1900,7 +1900,7 @@
         <v>3</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K5" s="14" t="s">
         <v>19</v>
@@ -1925,7 +1925,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D6" s="12">
         <v>111146</v>
@@ -1946,7 +1946,7 @@
         <v>3</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K6" s="14" t="s">
         <v>19</v>
@@ -1971,7 +1971,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" s="12">
         <v>111147</v>
@@ -1992,13 +1992,13 @@
         <v>3</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K7" s="14" t="s">
         <v>32</v>
       </c>
       <c r="L7" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M7" s="14" t="s">
         <v>45</v>
@@ -2017,7 +2017,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8" s="12">
         <v>111148</v>
@@ -2038,7 +2038,7 @@
         <v>3</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K8" s="14" t="s">
         <v>32</v>
@@ -2063,7 +2063,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" s="12">
         <v>111149</v>
@@ -2084,7 +2084,7 @@
         <v>3</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K9" s="14" t="s">
         <v>32</v>

</xml_diff>